<commit_message>
Esempi di riempimento automatico di celle
</commit_message>
<xml_diff>
--- a/Excel/Riempimento automatico.xlsx
+++ b/Excel/Riempimento automatico.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrea/Sviluppo/Didattica/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68E85E1-8170-754B-9528-77D011B36A99}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B546EC5-28B5-0A4F-98F1-174B63165FDA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{9B41355F-4DC6-DF40-A21B-5EB417024D60}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>Incremento unità:</t>
   </si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t>ESEMPI DI RIEMPIMENTO AUTOMATICO DI CELLE</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>Orari:</t>
+  </si>
+  <si>
+    <t>Incremento decimali:</t>
   </si>
 </sst>
 </file>
@@ -154,11 +163,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -473,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C01C120-0F2D-4046-9277-816F3062558E}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B11" sqref="B11:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -676,72 +687,177 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" t="s">
-        <v>8</v>
-      </c>
-      <c r="K7" t="s">
-        <v>9</v>
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>1.5</v>
+      </c>
+      <c r="C7">
+        <v>2.5</v>
+      </c>
+      <c r="D7">
+        <v>3.5</v>
+      </c>
+      <c r="E7">
+        <v>4.5</v>
+      </c>
+      <c r="F7">
+        <v>5.5</v>
+      </c>
+      <c r="G7">
+        <v>6.5</v>
+      </c>
+      <c r="H7">
+        <v>7.5</v>
+      </c>
+      <c r="I7">
+        <v>8.5</v>
+      </c>
+      <c r="J7">
+        <v>9.5</v>
+      </c>
+      <c r="K7">
+        <v>10.5</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>16</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>17</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>18</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>19</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G9" t="s">
         <v>20</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H9" t="s">
         <v>21</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I9" t="s">
         <v>22</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J9" t="s">
         <v>23</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K9" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="2">
+        <v>43160</v>
+      </c>
+      <c r="C10" s="2">
+        <v>43161</v>
+      </c>
+      <c r="D10" s="2">
+        <v>43162</v>
+      </c>
+      <c r="E10" s="2">
+        <v>43163</v>
+      </c>
+      <c r="F10" s="2">
+        <v>43164</v>
+      </c>
+      <c r="G10" s="2">
+        <v>43165</v>
+      </c>
+      <c r="H10" s="2">
+        <v>43166</v>
+      </c>
+      <c r="I10" s="2">
+        <v>43167</v>
+      </c>
+      <c r="J10" s="2">
+        <v>43168</v>
+      </c>
+      <c r="K10" s="2">
+        <v>43169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.27083333333333298</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.29166666666666702</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.3125</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.33333333333333398</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.35416666666666702</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.39583333333333398</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0.41666666666666702</v>
       </c>
     </row>
   </sheetData>

</xml_diff>